<commit_message>
start of variable costs
Includes working 'not blank' (second iteration)
</commit_message>
<xml_diff>
--- a/FRC_Assets/02_Fund_Raising_Calculator.xlsx
+++ b/FRC_Assets/02_Fund_Raising_Calculator.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://masseyhighschoolnz-my.sharepoint.com/personal/jgottschalk_masseyhigh_school_nz/Documents/Projects/01_Tutorials/12I_91896_7_v2_Adv_Programming_Revisited/91896_7_v2_support_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://masseyhighschoolnz-my.sharepoint.com/personal/jgottschalk_masseyhigh_school_nz/Documents/Projects/02_Tutorial_Answers/12_Advanced_Programming_Revisited/FRC_Panda/FRC_Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{812A805A-F43D-4689-A46B-BB5586C1D7C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1F075ED8-BFC2-49FF-8E95-B1985A4A2084}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="8_{812A805A-F43D-4689-A46B-BB5586C1D7C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5978B340-7A3A-44B3-A5B2-FC85D616DD62}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{74EEDAD5-0EF5-4421-8296-520D2E1E24A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{74EEDAD5-0EF5-4421-8296-520D2E1E24A8}"/>
   </bookViews>
   <sheets>
     <sheet name="$ Goal" sheetId="1" r:id="rId1"/>
     <sheet name="% Goal" sheetId="2" r:id="rId2"/>
+    <sheet name="variable costs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
   <si>
     <t>Item Name</t>
   </si>
@@ -80,15 +81,25 @@
   </si>
   <si>
     <t>Total Expenses</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -107,7 +118,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,8 +137,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -146,11 +163,79 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="7"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="7"/>
+      </right>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="7"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="7"/>
+      </right>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -166,6 +251,26 @@
     <xf numFmtId="8" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0B654C-E6B0-48F0-986E-7E78568DAFDE}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,4 +975,104 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82C5F60-9A70-4436-9063-2BAB77345F1C}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="212" zoomScaleNormal="212" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="22">
+        <v>300</v>
+      </c>
+      <c r="C4" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="D4" s="24">
+        <f>B4*C4</f>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="16">
+        <v>300</v>
+      </c>
+      <c r="C5" s="17">
+        <v>1</v>
+      </c>
+      <c r="D5" s="18">
+        <f t="shared" ref="D5:D6" si="0">B5*C5</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="26">
+        <v>50</v>
+      </c>
+      <c r="C6" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="28">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="12">
+        <f>SUM(D4:D6)</f>
+        <v>550</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
part way through selling price
</commit_message>
<xml_diff>
--- a/FRC_Assets/02_Fund_Raising_Calculator.xlsx
+++ b/FRC_Assets/02_Fund_Raising_Calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://masseyhighschoolnz-my.sharepoint.com/personal/jgottschalk_masseyhigh_school_nz/Documents/Projects/02_Tutorial_Answers/12_Advanced_Programming_Revisited/FRC_Panda/FRC_Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="8_{812A805A-F43D-4689-A46B-BB5586C1D7C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ADBB80BE-0059-49E1-9399-87562B1591B1}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="8_{812A805A-F43D-4689-A46B-BB5586C1D7C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EC3CBAFD-DFE4-4AFD-9E9A-A59A2150CE73}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{74EEDAD5-0EF5-4421-8296-520D2E1E24A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{74EEDAD5-0EF5-4421-8296-520D2E1E24A8}"/>
   </bookViews>
   <sheets>
     <sheet name="$ Goal" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="variable costs" sheetId="3" r:id="rId3"/>
     <sheet name="fixed costs" sheetId="4" r:id="rId4"/>
     <sheet name="fixed_variable" sheetId="5" r:id="rId5"/>
+    <sheet name="Selling Price" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="25">
   <si>
     <t>Item Name</t>
   </si>
@@ -95,6 +96,24 @@
   </si>
   <si>
     <t>Item</t>
+  </si>
+  <si>
+    <t># of items</t>
+  </si>
+  <si>
+    <t>Total Costs</t>
+  </si>
+  <si>
+    <t>Price / item</t>
+  </si>
+  <si>
+    <t>Round to</t>
+  </si>
+  <si>
+    <t>Suggested Price</t>
+  </si>
+  <si>
+    <t>Profit goal ($)</t>
   </si>
 </sst>
 </file>
@@ -551,15 +570,15 @@
     <xf numFmtId="8" fontId="0" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="8" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -877,7 +896,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D15"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1428,8 +1447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A27EAA53-FD95-4E32-921A-6C66E3D505AD}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD13"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,12 +1459,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
       <c r="E1" s="31"/>
       <c r="F1" s="13" t="s">
         <v>2</v>
@@ -1604,12 +1623,12 @@
       <c r="J7" s="31"/>
     </row>
     <row r="8" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
       <c r="E8" s="31"/>
       <c r="F8" s="13" t="s">
         <v>14</v>
@@ -1722,12 +1741,12 @@
       <c r="J14" s="31"/>
     </row>
     <row r="15" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="72" t="s">
+      <c r="A15" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="73"/>
-      <c r="C15" s="73"/>
-      <c r="D15" s="74">
+      <c r="B15" s="71"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="72">
         <f>D6</f>
         <v>675</v>
       </c>
@@ -1782,4 +1801,67 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB96C055-CB23-41B9-9888-A60D4F6D369B}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>50</v>
+      </c>
+      <c r="B2">
+        <v>200</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <f>(B2+C2)/A2</f>
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Complete outcome (pre final checks)
</commit_message>
<xml_diff>
--- a/FRC_Assets/02_Fund_Raising_Calculator.xlsx
+++ b/FRC_Assets/02_Fund_Raising_Calculator.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://masseyhighschoolnz-my.sharepoint.com/personal/jgottschalk_masseyhigh_school_nz/Documents/Projects/02_Tutorial_Answers/12_Advanced_Programming_Revisited/FRC_Panda/FRC_Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="173" documentId="8_{812A805A-F43D-4689-A46B-BB5586C1D7C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6ADDA2DC-4E33-4057-9AFD-8D44ECDBFECC}"/>
+  <xr:revisionPtr revIDLastSave="272" documentId="8_{812A805A-F43D-4689-A46B-BB5586C1D7C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{57E2EC1A-5C12-47BC-B7B2-B37B6CF0E11F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{74EEDAD5-0EF5-4421-8296-520D2E1E24A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{74EEDAD5-0EF5-4421-8296-520D2E1E24A8}"/>
   </bookViews>
   <sheets>
-    <sheet name="$ Goal" sheetId="1" r:id="rId1"/>
-    <sheet name="% Goal" sheetId="2" r:id="rId2"/>
-    <sheet name="variable costs" sheetId="3" r:id="rId3"/>
-    <sheet name="fixed costs" sheetId="4" r:id="rId4"/>
-    <sheet name="fixed_variable" sheetId="5" r:id="rId5"/>
-    <sheet name="Selling Price" sheetId="6" r:id="rId6"/>
+    <sheet name="no_fixed" sheetId="7" r:id="rId1"/>
+    <sheet name="$ Goal" sheetId="1" r:id="rId2"/>
+    <sheet name="% Goal" sheetId="2" r:id="rId3"/>
+    <sheet name="variable costs" sheetId="3" r:id="rId4"/>
+    <sheet name="fixed costs" sheetId="4" r:id="rId5"/>
+    <sheet name="fixed_variable" sheetId="5" r:id="rId6"/>
+    <sheet name="Selling Price" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="26">
   <si>
     <t>Item Name</t>
   </si>
@@ -118,6 +119,9 @@
   <si>
     <t># of
 items</t>
+  </si>
+  <si>
+    <t>Amount</t>
   </si>
 </sst>
 </file>
@@ -177,7 +181,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,8 +242,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor theme="5" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFBDBD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -493,11 +533,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -507,7 +596,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="8" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -577,72 +665,118 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="8" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="11" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="11" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="3" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="3" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="3" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
+    <xf numFmtId="6" fontId="3" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
+    <xf numFmtId="8" fontId="3" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
+    <xf numFmtId="8" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
+    <xf numFmtId="8" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFBDBD"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -950,201 +1084,402 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46301BA7-176A-4F23-93AD-62F786FF0F36}">
-  <dimension ref="A1:E20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C2B07B-40C0-4305-85C3-D04AA53EE7C2}">
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1">
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1">
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B5" s="46">
         <v>0.75</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C5" s="47">
         <v>300</v>
       </c>
-      <c r="D4" s="5">
-        <f>C4*B4</f>
+      <c r="D5" s="36">
+        <f>C5*B5</f>
         <v>225</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B6" s="48">
         <v>1</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C6" s="49">
         <v>300</v>
       </c>
-      <c r="D5" s="5">
-        <f t="shared" ref="D5:D6" si="0">C5*B5</f>
+      <c r="D6" s="38">
+        <f t="shared" ref="D6:D7" si="0">C6*B6</f>
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B7" s="51">
         <v>0.5</v>
       </c>
-      <c r="C6" s="4">
-        <v>300</v>
-      </c>
-      <c r="D6" s="5">
+      <c r="C7" s="52">
+        <v>100</v>
+      </c>
+      <c r="D7" s="53">
         <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="12">
-        <f>SUM(D4:D6)</f>
-        <v>675</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="8">
-        <v>25</v>
-      </c>
-      <c r="C10" s="7">
-        <v>1</v>
-      </c>
-      <c r="D10" s="8">
-        <f>C10*B10</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="8">
-        <v>35</v>
-      </c>
-      <c r="C11" s="7">
-        <v>1</v>
-      </c>
-      <c r="D11" s="8">
-        <f t="shared" ref="D11:D12" si="1">C11*B11</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="8">
-        <v>15</v>
-      </c>
-      <c r="C12" s="7">
-        <v>1</v>
-      </c>
-      <c r="D12" s="8">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="11">
-        <f>SUM(D10:D12)</f>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="30"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="106">
+        <f>SUM(D5:D7)</f>
+        <v>575</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+    </row>
+    <row r="10" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="109" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="10">
-        <f>D7+D13</f>
-        <v>750</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="B10" s="109"/>
+      <c r="C10" s="109"/>
+      <c r="D10" s="108">
+        <f>D8</f>
+        <v>575</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="30" customFormat="1" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="116"/>
+      <c r="B11" s="116"/>
+      <c r="C11" s="116"/>
+      <c r="D11" s="117"/>
+    </row>
+    <row r="12" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="9">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="B12" s="110"/>
+      <c r="C12" s="110"/>
+      <c r="D12" s="118">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="110"/>
+      <c r="B13" s="110"/>
+      <c r="C13" s="110"/>
+      <c r="D13" s="111">
+        <f>D12*D10+D10</f>
+        <v>862.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="2">
-        <f>(B17+D15)/E1</f>
+      <c r="B15" s="112"/>
+      <c r="C15" s="112"/>
+      <c r="D15" s="113">
+        <f>(D13+D10)/D1</f>
+        <v>4.791666666666667</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="114" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="114"/>
+      <c r="C16" s="114"/>
+      <c r="D16" s="115">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="2">
-        <v>5.75</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A12:C12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46301BA7-176A-4F23-93AD-62F786FF0F36}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="92" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="93" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="46">
+        <v>0.75</v>
+      </c>
+      <c r="C5" s="47">
+        <v>300</v>
+      </c>
+      <c r="D5" s="36">
+        <f>C5*B5</f>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="48">
+        <v>1</v>
+      </c>
+      <c r="C6" s="49">
+        <v>300</v>
+      </c>
+      <c r="D6" s="38">
+        <f t="shared" ref="D6:D7" si="0">C6*B6</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="51">
+        <v>0.5</v>
+      </c>
+      <c r="C7" s="52">
+        <v>100</v>
+      </c>
+      <c r="D7" s="53">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="30"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="106">
+        <f>SUM(D5:D7)</f>
+        <v>575</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+    </row>
+    <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B10" s="105" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="105"/>
+      <c r="D10" s="105"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="94" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="95"/>
+      <c r="D11" s="95" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="96" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="97"/>
+      <c r="D12" s="98">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="99" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="100"/>
+      <c r="D13" s="101">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="102" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="103"/>
+      <c r="D14" s="104">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="107">
+        <f>SUM(D12:D14)</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="109" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="109"/>
+      <c r="C17" s="109"/>
+      <c r="D17" s="108">
+        <f>D8+D15</f>
+        <v>650</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="110" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="110"/>
+      <c r="C19" s="110"/>
+      <c r="D19" s="111">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="112" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="112"/>
+      <c r="C21" s="112"/>
+      <c r="D21" s="113">
+        <f>(D19+D17)/D1</f>
+        <v>4.666666666666667</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="114" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="114"/>
+      <c r="C22" s="114"/>
+      <c r="D22" s="115">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A21:C21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0B654C-E6B0-48F0-986E-7E78568DAFDE}">
   <dimension ref="A1:E20"/>
   <sheetViews>
@@ -1229,7 +1564,7 @@
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <f>SUM(D4:D6)</f>
         <v>675</v>
       </c>
@@ -1292,17 +1627,17 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="7"/>
-      <c r="D13" s="11">
+      <c r="D13" s="10">
         <f>SUM(D10:D12)</f>
         <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="9">
         <f>D7+D13</f>
         <v>750</v>
       </c>
@@ -1312,7 +1647,7 @@
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="13">
         <v>0.75</v>
       </c>
       <c r="D17" s="2">
@@ -1343,7 +1678,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82C5F60-9A70-4436-9063-2BAB77345F1C}">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -1369,60 +1704,60 @@
       <c r="C1" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="29" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="21">
         <v>300</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="22">
         <v>0.75</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <f>B4*C4</f>
         <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="15">
         <v>300</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="16">
         <v>1</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <f t="shared" ref="D5:D6" si="0">B5*C5</f>
         <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="25">
         <v>50</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="26">
         <v>0.5</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="27">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
@@ -1431,7 +1766,7 @@
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <f>SUM(D4:D6)</f>
         <v>550</v>
       </c>
@@ -1443,7 +1778,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4049CE12-8D15-461A-A234-77ACB9C2534A}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1457,40 +1792,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="34" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="37">
+      <c r="B2" s="36">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="39">
+      <c r="B3" s="38">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="37">
+      <c r="B4" s="36">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
-      <c r="B5" s="41">
+      <c r="A5" s="39"/>
+      <c r="B5" s="40">
         <f>SUM(B2:B4)</f>
         <v>75</v>
       </c>
@@ -1501,7 +1836,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A27EAA53-FD95-4E32-921A-6C66E3D505AD}">
   <dimension ref="A1:J18"/>
   <sheetViews>
@@ -1517,339 +1852,339 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="13" t="s">
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="44" t="s">
+      <c r="E2" s="30"/>
+      <c r="F2" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="31"/>
+      <c r="J2" s="30"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="47">
+      <c r="B3" s="46">
         <v>0.75</v>
       </c>
-      <c r="C3" s="48">
+      <c r="C3" s="47">
         <v>300</v>
       </c>
-      <c r="D3" s="37">
+      <c r="D3" s="36">
         <f>C3*B3</f>
         <v>225</v>
       </c>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31" t="s">
+      <c r="E3" s="30"/>
+      <c r="F3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="32">
+      <c r="G3" s="31">
         <v>0.75</v>
       </c>
-      <c r="H3" s="31">
+      <c r="H3" s="30">
         <v>300</v>
       </c>
-      <c r="I3" s="32">
+      <c r="I3" s="31">
         <f>H3*G3</f>
         <v>225</v>
       </c>
-      <c r="J3" s="31"/>
+      <c r="J3" s="30"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="49">
+      <c r="B4" s="48">
         <v>1</v>
       </c>
-      <c r="C4" s="50">
+      <c r="C4" s="49">
         <v>300</v>
       </c>
-      <c r="D4" s="39">
+      <c r="D4" s="38">
         <f t="shared" ref="D4:D5" si="0">C4*B4</f>
         <v>300</v>
       </c>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31" t="s">
+      <c r="E4" s="30"/>
+      <c r="F4" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="32">
+      <c r="G4" s="31">
         <v>1</v>
       </c>
-      <c r="H4" s="31">
+      <c r="H4" s="30">
         <v>300</v>
       </c>
-      <c r="I4" s="32">
+      <c r="I4" s="31">
         <f t="shared" ref="I4:I5" si="1">H4*G4</f>
         <v>300</v>
       </c>
-      <c r="J4" s="31"/>
+      <c r="J4" s="30"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="52">
+      <c r="B5" s="51">
         <v>0.5</v>
       </c>
-      <c r="C5" s="53">
+      <c r="C5" s="52">
         <v>300</v>
       </c>
-      <c r="D5" s="54">
+      <c r="D5" s="53">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31" t="s">
+      <c r="E5" s="30"/>
+      <c r="F5" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="32">
+      <c r="G5" s="31">
         <v>0.5</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="30">
         <v>300</v>
       </c>
-      <c r="I5" s="32">
+      <c r="I5" s="31">
         <f t="shared" si="1"/>
         <v>150</v>
       </c>
-      <c r="J5" s="31"/>
+      <c r="J5" s="30"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="31"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="33">
+      <c r="A6" s="30"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="32">
         <f>SUM(D3:D5)</f>
         <v>675</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="33">
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="32">
         <f>SUM(I3:I5)</f>
         <v>675</v>
       </c>
-      <c r="J6" s="31"/>
+      <c r="J6" s="30"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
     </row>
     <row r="8" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="73" t="s">
+      <c r="A8" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="13" t="s">
+      <c r="B8" s="90"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="42">
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="41">
         <f>I6</f>
         <v>675</v>
       </c>
-      <c r="J8" s="31"/>
+      <c r="J8" s="30"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="55" t="s">
+      <c r="A9" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="57" t="s">
+      <c r="C9" s="55"/>
+      <c r="D9" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="31"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="30"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="59">
+      <c r="B10" s="58">
         <v>25</v>
       </c>
-      <c r="C10" s="60"/>
-      <c r="D10" s="61">
+      <c r="C10" s="59"/>
+      <c r="D10" s="60">
         <v>25</v>
       </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="63">
+      <c r="B11" s="62">
         <v>35</v>
       </c>
-      <c r="C11" s="64"/>
-      <c r="D11" s="65">
+      <c r="C11" s="63"/>
+      <c r="D11" s="64">
         <v>35</v>
       </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="66" t="s">
+      <c r="A12" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="67">
+      <c r="B12" s="66">
         <v>15</v>
       </c>
-      <c r="C12" s="68"/>
-      <c r="D12" s="69">
+      <c r="C12" s="67"/>
+      <c r="D12" s="68">
         <v>15</v>
       </c>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="31"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="33">
+      <c r="A13" s="30"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="32">
         <f>SUM(D10:D12)</f>
         <v>75</v>
       </c>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
     </row>
     <row r="15" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="70" t="s">
+      <c r="A15" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="71"/>
-      <c r="C15" s="71"/>
-      <c r="D15" s="72">
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="71">
         <f>D6</f>
         <v>675</v>
       </c>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1861,106 +2196,106 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB96C055-CB23-41B9-9888-A60D4F6D369B}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="262" zoomScaleNormal="262" workbookViewId="0">
+    <sheetView zoomScale="262" zoomScaleNormal="262" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="83" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="7.5703125" style="83" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="83" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" style="83" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="83" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="83"/>
+    <col min="1" max="1" width="9.7109375" style="80" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7.5703125" style="80" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="80" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" style="80" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="80" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="80"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="92" t="s">
+    <row r="1" spans="1:6" s="75" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="76" t="s">
+      <c r="E1" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="F1" s="74" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="79">
+      <c r="A2" s="76">
         <v>50</v>
       </c>
-      <c r="B2" s="81">
+      <c r="B2" s="78">
         <v>45.5</v>
       </c>
-      <c r="C2" s="80">
+      <c r="C2" s="77">
         <v>100</v>
       </c>
-      <c r="D2" s="81">
+      <c r="D2" s="78">
         <f>(B2+C2)/A2</f>
         <v>2.91</v>
       </c>
-      <c r="E2" s="80">
+      <c r="E2" s="77">
         <v>1</v>
       </c>
-      <c r="F2" s="82">
+      <c r="F2" s="79">
         <f>CEILING(D2,E2)</f>
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="84">
+      <c r="A3" s="81">
         <v>50</v>
       </c>
-      <c r="B3" s="86">
+      <c r="B3" s="83">
         <v>105</v>
       </c>
-      <c r="C3" s="85">
+      <c r="C3" s="82">
         <v>100</v>
       </c>
-      <c r="D3" s="86">
+      <c r="D3" s="83">
         <f>(B3+C3)/A3</f>
         <v>4.0999999999999996</v>
       </c>
-      <c r="E3" s="85">
+      <c r="E3" s="82">
         <v>1</v>
       </c>
-      <c r="F3" s="87">
+      <c r="F3" s="84">
         <f>CEILING(D3,E3)</f>
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="88">
+      <c r="A4" s="85">
         <v>50</v>
       </c>
-      <c r="B4" s="90">
+      <c r="B4" s="87">
         <v>200</v>
       </c>
-      <c r="C4" s="89">
+      <c r="C4" s="86">
         <v>100</v>
       </c>
-      <c r="D4" s="90">
+      <c r="D4" s="87">
         <f>(B4+C4)/A4</f>
         <v>6</v>
       </c>
-      <c r="E4" s="89">
+      <c r="E4" s="86">
         <v>5</v>
       </c>
-      <c r="F4" s="91">
+      <c r="F4" s="88">
         <f>CEILING(D4,E4)</f>
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Minor changes to component code
Mostly getting rid of PEP 8 errors whilst creating video tutorials
</commit_message>
<xml_diff>
--- a/FRC_Assets/02_Fund_Raising_Calculator.xlsx
+++ b/FRC_Assets/02_Fund_Raising_Calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://masseyhighschoolnz-my.sharepoint.com/personal/jgottschalk_masseyhigh_school_nz/Documents/Projects/02_Tutorial_Answers/12_Advanced_Programming_Revisited/FRC_Panda/FRC_Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="275" documentId="8_{812A805A-F43D-4689-A46B-BB5586C1D7C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{99A25771-415D-43AF-9611-89811FA6D665}"/>
+  <xr:revisionPtr revIDLastSave="286" documentId="8_{812A805A-F43D-4689-A46B-BB5586C1D7C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9B333353-0CE2-46D4-8748-5690FA1B7431}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{74EEDAD5-0EF5-4421-8296-520D2E1E24A8}"/>
+    <workbookView xWindow="4590" yWindow="570" windowWidth="15375" windowHeight="7875" firstSheet="2" activeTab="3" xr2:uid="{74EEDAD5-0EF5-4421-8296-520D2E1E24A8}"/>
   </bookViews>
   <sheets>
     <sheet name="$ Goal" sheetId="1" r:id="rId1"/>
@@ -279,7 +279,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -299,26 +299,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="7"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="7"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="7"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color theme="7"/>
@@ -327,43 +307,6 @@
         <color theme="7"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="7"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="7"/>
-      </top>
-      <bottom style="thin">
-        <color theme="7"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="7"/>
-      </top>
-      <bottom style="thin">
-        <color theme="7"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="7"/>
-      </right>
-      <top style="thin">
-        <color theme="7"/>
-      </top>
-      <bottom style="thin">
-        <color theme="7"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -586,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -601,136 +544,116 @@
     <xf numFmtId="8" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="8" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="11" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="11" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="11" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="11" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="3" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="3" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="3" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -742,9 +665,26 @@
     </xf>
     <xf numFmtId="8" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
@@ -754,16 +694,10 @@
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1099,7 +1033,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="74" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -1110,179 +1044,179 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="111" t="s">
+      <c r="A3" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="111"/>
-      <c r="C3" s="111"/>
-      <c r="D3" s="111"/>
+      <c r="B3" s="103"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="29" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="46">
+      <c r="B5" s="30">
         <v>0.75</v>
       </c>
-      <c r="C5" s="47">
-        <v>300</v>
-      </c>
-      <c r="D5" s="36">
+      <c r="C5" s="31">
+        <v>300</v>
+      </c>
+      <c r="D5" s="20">
         <f>C5*B5</f>
         <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="48">
+      <c r="B6" s="32">
         <v>1</v>
       </c>
-      <c r="C6" s="49">
-        <v>300</v>
-      </c>
-      <c r="D6" s="38">
+      <c r="C6" s="33">
+        <v>300</v>
+      </c>
+      <c r="D6" s="22">
         <f t="shared" ref="D6:D7" si="0">C6*B6</f>
         <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="51">
+      <c r="B7" s="35">
         <v>0.5</v>
       </c>
-      <c r="C7" s="52">
+      <c r="C7" s="36">
         <v>100</v>
       </c>
-      <c r="D7" s="53">
+      <c r="D7" s="37">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="30"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="102">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="86">
         <f>SUM(D5:D7)</f>
         <v>575</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
     </row>
     <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B10" s="116" t="s">
+      <c r="B10" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="116"/>
-      <c r="D10" s="116"/>
+      <c r="C10" s="104"/>
+      <c r="D10" s="104"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="91" t="s">
+      <c r="B11" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="92"/>
-      <c r="D11" s="92" t="s">
+      <c r="C11" s="76"/>
+      <c r="D11" s="76" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="93" t="s">
+      <c r="B12" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="94"/>
-      <c r="D12" s="95">
+      <c r="C12" s="78"/>
+      <c r="D12" s="79">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="96" t="s">
+      <c r="B13" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="97"/>
-      <c r="D13" s="98">
+      <c r="C13" s="81"/>
+      <c r="D13" s="82">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="99" t="s">
+      <c r="B14" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="100"/>
-      <c r="D14" s="101">
+      <c r="C14" s="84"/>
+      <c r="D14" s="85">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="103">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="87">
         <f>SUM(D12:D14)</f>
         <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="112" t="s">
+      <c r="A17" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="112"/>
-      <c r="C17" s="112"/>
-      <c r="D17" s="104">
+      <c r="B17" s="105"/>
+      <c r="C17" s="105"/>
+      <c r="D17" s="88">
         <f>D8+D15</f>
         <v>650</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="113" t="s">
+      <c r="A19" s="106" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="113"/>
-      <c r="C19" s="113"/>
-      <c r="D19" s="105">
+      <c r="B19" s="106"/>
+      <c r="C19" s="106"/>
+      <c r="D19" s="89">
         <v>750</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="114" t="s">
+      <c r="A21" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="114"/>
-      <c r="C21" s="114"/>
-      <c r="D21" s="106">
+      <c r="B21" s="107"/>
+      <c r="C21" s="107"/>
+      <c r="D21" s="90">
         <f>(D19+D17)/D1</f>
         <v>4.666666666666667</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="115" t="s">
+      <c r="A22" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="115"/>
-      <c r="C22" s="115"/>
-      <c r="D22" s="107">
+      <c r="B22" s="102"/>
+      <c r="C22" s="102"/>
+      <c r="D22" s="91">
         <v>5</v>
       </c>
     </row>
@@ -1304,7 +1238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C2B07B-40C0-4305-85C3-D04AA53EE7C2}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -1316,7 +1250,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="74" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -1327,141 +1261,141 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="111" t="s">
+      <c r="A3" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="111"/>
-      <c r="C3" s="111"/>
-      <c r="D3" s="111"/>
+      <c r="B3" s="103"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="29" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="46">
+      <c r="B5" s="30">
         <v>0.75</v>
       </c>
-      <c r="C5" s="47">
-        <v>300</v>
-      </c>
-      <c r="D5" s="36">
+      <c r="C5" s="31">
+        <v>300</v>
+      </c>
+      <c r="D5" s="20">
         <f>C5*B5</f>
         <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="48">
+      <c r="B6" s="32">
         <v>1</v>
       </c>
-      <c r="C6" s="49">
-        <v>300</v>
-      </c>
-      <c r="D6" s="38">
+      <c r="C6" s="33">
+        <v>300</v>
+      </c>
+      <c r="D6" s="22">
         <f t="shared" ref="D6:D7" si="0">C6*B6</f>
         <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="51">
+      <c r="B7" s="35">
         <v>0.5</v>
       </c>
-      <c r="C7" s="52">
+      <c r="C7" s="36">
         <v>100</v>
       </c>
-      <c r="D7" s="53">
+      <c r="D7" s="37">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="30"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="102">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="86">
         <f>SUM(D5:D7)</f>
         <v>575</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
     </row>
     <row r="10" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="112" t="s">
+      <c r="A10" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="112"/>
-      <c r="C10" s="112"/>
-      <c r="D10" s="104">
+      <c r="B10" s="105"/>
+      <c r="C10" s="105"/>
+      <c r="D10" s="88">
         <f>D8</f>
         <v>575</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="30" customFormat="1" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="108"/>
-      <c r="B11" s="108"/>
-      <c r="C11" s="108"/>
-      <c r="D11" s="109"/>
+    <row r="11" spans="1:4" s="14" customFormat="1" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="92"/>
+      <c r="B11" s="92"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="93"/>
     </row>
     <row r="12" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="113" t="s">
+      <c r="A12" s="106" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="113"/>
-      <c r="C12" s="113"/>
-      <c r="D12" s="110">
+      <c r="B12" s="106"/>
+      <c r="C12" s="106"/>
+      <c r="D12" s="94">
         <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="113"/>
-      <c r="B13" s="113"/>
-      <c r="C13" s="113"/>
-      <c r="D13" s="105">
+      <c r="A13" s="106"/>
+      <c r="B13" s="106"/>
+      <c r="C13" s="106"/>
+      <c r="D13" s="89">
         <f>D12*D10+D10</f>
         <v>862.5</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="114" t="s">
+      <c r="A15" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="114"/>
-      <c r="C15" s="114"/>
-      <c r="D15" s="106">
+      <c r="B15" s="107"/>
+      <c r="C15" s="107"/>
+      <c r="D15" s="90">
         <f>(D13)/D1</f>
         <v>2.875</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="115" t="s">
+      <c r="A16" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="115"/>
-      <c r="C16" s="115"/>
-      <c r="D16" s="107">
+      <c r="B16" s="102"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="91">
         <v>3</v>
       </c>
     </row>
@@ -1680,21 +1614,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82C5F60-9A70-4436-9063-2BAB77345F1C}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScale="212" zoomScaleNormal="212" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D3"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1703,75 +1637,100 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="98" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="E3" s="95"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="21">
-        <v>300</v>
-      </c>
-      <c r="C4" s="22">
+      <c r="B4" s="99">
+        <v>300</v>
+      </c>
+      <c r="C4" s="30">
         <v>0.75</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="20">
         <f>B4*C4</f>
         <v>225</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="E4" s="95"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="15">
-        <v>300</v>
-      </c>
-      <c r="C5" s="16">
+      <c r="B5" s="100">
+        <v>300</v>
+      </c>
+      <c r="C5" s="32">
         <v>1</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="22">
         <f t="shared" ref="D5:D6" si="0">B5*C5</f>
         <v>300</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="E5" s="95"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="101">
         <v>50</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="35">
         <v>0.5</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="37">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="11">
+      <c r="E6" s="95"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="95"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="96">
         <f>SUM(D4:D6)</f>
         <v>550</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="E7" s="95"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="95"/>
+      <c r="B8" s="95"/>
+      <c r="C8" s="95"/>
+      <c r="D8" s="95"/>
+      <c r="E8" s="95"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="95"/>
+      <c r="B9" s="95"/>
+      <c r="C9" s="95"/>
+      <c r="D9" s="95"/>
+      <c r="E9" s="95"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="95"/>
+      <c r="B10" s="95"/>
+      <c r="C10" s="95"/>
+      <c r="D10" s="95"/>
+      <c r="E10" s="95"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1792,40 +1751,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="18" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="36">
+      <c r="B2" s="20">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="38">
+      <c r="B3" s="22">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="36">
+      <c r="B4" s="20">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="39"/>
-      <c r="B5" s="40">
+      <c r="A5" s="23"/>
+      <c r="B5" s="24">
         <f>SUM(B2:B4)</f>
         <v>75</v>
       </c>
@@ -1852,339 +1811,339 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="30"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="14"/>
       <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="43" t="s">
+      <c r="E2" s="14"/>
+      <c r="F2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="30" t="s">
+      <c r="I2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="30"/>
+      <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="46">
+      <c r="B3" s="30">
         <v>0.75</v>
       </c>
-      <c r="C3" s="47">
-        <v>300</v>
-      </c>
-      <c r="D3" s="36">
+      <c r="C3" s="31">
+        <v>300</v>
+      </c>
+      <c r="D3" s="20">
         <f>C3*B3</f>
         <v>225</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30" t="s">
+      <c r="E3" s="14"/>
+      <c r="F3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="31">
+      <c r="G3" s="15">
         <v>0.75</v>
       </c>
-      <c r="H3" s="30">
-        <v>300</v>
-      </c>
-      <c r="I3" s="31">
+      <c r="H3" s="14">
+        <v>300</v>
+      </c>
+      <c r="I3" s="15">
         <f>H3*G3</f>
         <v>225</v>
       </c>
-      <c r="J3" s="30"/>
+      <c r="J3" s="14"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="48">
+      <c r="B4" s="32">
         <v>1</v>
       </c>
-      <c r="C4" s="49">
-        <v>300</v>
-      </c>
-      <c r="D4" s="38">
+      <c r="C4" s="33">
+        <v>300</v>
+      </c>
+      <c r="D4" s="22">
         <f t="shared" ref="D4:D5" si="0">C4*B4</f>
         <v>300</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30" t="s">
+      <c r="E4" s="14"/>
+      <c r="F4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="15">
         <v>1</v>
       </c>
-      <c r="H4" s="30">
-        <v>300</v>
-      </c>
-      <c r="I4" s="31">
+      <c r="H4" s="14">
+        <v>300</v>
+      </c>
+      <c r="I4" s="15">
         <f t="shared" ref="I4:I5" si="1">H4*G4</f>
         <v>300</v>
       </c>
-      <c r="J4" s="30"/>
+      <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="51">
+      <c r="B5" s="35">
         <v>0.5</v>
       </c>
-      <c r="C5" s="52">
-        <v>300</v>
-      </c>
-      <c r="D5" s="53">
+      <c r="C5" s="36">
+        <v>300</v>
+      </c>
+      <c r="D5" s="37">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30" t="s">
+      <c r="E5" s="14"/>
+      <c r="F5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="15">
         <v>0.5</v>
       </c>
-      <c r="H5" s="30">
-        <v>300</v>
-      </c>
-      <c r="I5" s="31">
+      <c r="H5" s="14">
+        <v>300</v>
+      </c>
+      <c r="I5" s="15">
         <f t="shared" si="1"/>
         <v>150</v>
       </c>
-      <c r="J5" s="30"/>
+      <c r="J5" s="14"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="32">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="16">
         <f>SUM(D3:D5)</f>
         <v>675</v>
       </c>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="32">
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="16">
         <f>SUM(I3:I5)</f>
         <v>675</v>
       </c>
-      <c r="J6" s="30"/>
+      <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
     </row>
     <row r="8" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="117" t="s">
+      <c r="A8" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="117"/>
-      <c r="C8" s="117"/>
-      <c r="D8" s="117"/>
-      <c r="E8" s="30"/>
+      <c r="B8" s="108"/>
+      <c r="C8" s="108"/>
+      <c r="D8" s="108"/>
+      <c r="E8" s="14"/>
       <c r="F8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="41">
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="25">
         <f>I6</f>
         <v>675</v>
       </c>
-      <c r="J8" s="30"/>
+      <c r="J8" s="14"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="54" t="s">
+      <c r="A9" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="55"/>
-      <c r="D9" s="56" t="s">
+      <c r="C9" s="39"/>
+      <c r="D9" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="30"/>
+      <c r="E9" s="14"/>
       <c r="F9" s="12"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="30"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="14"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="58">
+      <c r="B10" s="42">
         <v>25</v>
       </c>
-      <c r="C10" s="59"/>
-      <c r="D10" s="60">
+      <c r="C10" s="43"/>
+      <c r="D10" s="44">
         <v>25</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="61" t="s">
+      <c r="A11" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="62">
+      <c r="B11" s="46">
         <v>35</v>
       </c>
-      <c r="C11" s="63"/>
-      <c r="D11" s="64">
+      <c r="C11" s="47"/>
+      <c r="D11" s="48">
         <v>35</v>
       </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="66">
+      <c r="B12" s="50">
         <v>15</v>
       </c>
-      <c r="C12" s="67"/>
-      <c r="D12" s="68">
+      <c r="C12" s="51"/>
+      <c r="D12" s="52">
         <v>15</v>
       </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="32">
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="16">
         <f>SUM(D10:D12)</f>
         <v>75</v>
       </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
     </row>
     <row r="15" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="69" t="s">
+      <c r="A15" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="70"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="71">
+      <c r="B15" s="54"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="55">
         <f>D6</f>
         <v>675</v>
       </c>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2206,96 +2165,96 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="80" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="7.5703125" style="80" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="80" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" style="80" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="80" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="80"/>
+    <col min="1" max="1" width="9.7109375" style="64" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7.5703125" style="64" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="64" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" style="64" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="64" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="64"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="75" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
+    <row r="1" spans="1:6" s="59" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="73" t="s">
+      <c r="D1" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="73" t="s">
+      <c r="E1" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="74" t="s">
+      <c r="F1" s="58" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="76">
+      <c r="A2" s="60">
         <v>50</v>
       </c>
-      <c r="B2" s="78">
+      <c r="B2" s="62">
         <v>45.5</v>
       </c>
-      <c r="C2" s="77">
+      <c r="C2" s="61">
         <v>100</v>
       </c>
-      <c r="D2" s="78">
+      <c r="D2" s="62">
         <f>(B2+C2)/A2</f>
         <v>2.91</v>
       </c>
-      <c r="E2" s="77">
+      <c r="E2" s="61">
         <v>1</v>
       </c>
-      <c r="F2" s="79">
+      <c r="F2" s="63">
         <f>CEILING(D2,E2)</f>
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="81">
+      <c r="A3" s="65">
         <v>50</v>
       </c>
-      <c r="B3" s="83">
+      <c r="B3" s="67">
         <v>105</v>
       </c>
-      <c r="C3" s="82">
+      <c r="C3" s="66">
         <v>100</v>
       </c>
-      <c r="D3" s="83">
+      <c r="D3" s="67">
         <f>(B3+C3)/A3</f>
         <v>4.0999999999999996</v>
       </c>
-      <c r="E3" s="82">
+      <c r="E3" s="66">
         <v>1</v>
       </c>
-      <c r="F3" s="84">
+      <c r="F3" s="68">
         <f>CEILING(D3,E3)</f>
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="85">
+      <c r="A4" s="69">
         <v>50</v>
       </c>
-      <c r="B4" s="87">
+      <c r="B4" s="71">
         <v>200</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="70">
         <v>100</v>
       </c>
-      <c r="D4" s="87">
+      <c r="D4" s="71">
         <f>(B4+C4)/A4</f>
         <v>6</v>
       </c>
-      <c r="E4" s="86">
+      <c r="E4" s="70">
         <v>5</v>
       </c>
-      <c r="F4" s="88">
+      <c r="F4" s="72">
         <f>CEILING(D4,E4)</f>
         <v>10</v>
       </c>

</xml_diff>